<commit_message>
Permission Processing On Api
</commit_message>
<xml_diff>
--- a/vertx-pin/zero-ambient/src/main/resources/plugin/ambient/oob/cab/system.document.xlsx
+++ b/vertx-pin/zero-ambient/src/main/resources/plugin/ambient/oob/cab/system.document.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lang/Develop/Source/ox-workshop/vertx-zero/vertx-pin/zero-ambient/src/main/resources/plugin/ambient/oob/cab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3970B2E-367E-E74F-BBBD-D363A49A53A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789A8672-7DBA-0241-BAA1-4E83BFC6B80D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41500" yWindow="-2980" windowWidth="51760" windowHeight="27280" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
+    <workbookView xWindow="53340" yWindow="-12160" windowWidth="41000" windowHeight="37860" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA-PERM" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="168">
   <si>
     <t>key</t>
   </si>
@@ -368,6 +368,260 @@
   </si>
   <si>
     <t>modeGroup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>res.file.upload</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x.attachment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>res.file.download</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4e7c30c2-c04e-4b2e-82dd-a2e3ebf54586</t>
+  </si>
+  <si>
+    <t>perm.file.download</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>51da4f23-2d92-40fc-a0b6-48f2ff3509db</t>
+  </si>
+  <si>
+    <t>perm.file.upload</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4b398ad8-0d8c-4dab-8954-85130b86d973</t>
+  </si>
+  <si>
+    <t>上传</t>
+  </si>
+  <si>
+    <t>7240209a-22d8-4ce5-a8a3-108c177354d9</t>
+  </si>
+  <si>
+    <t>下载</t>
+  </si>
+  <si>
+    <t>act.file.upload</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>/api/file/upload/:identifier</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>act.file.download</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/file/download/:fileKey</t>
+  </si>
+  <si>
+    <t>perm.document.trash</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>系统数据管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>perm.document.purge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1a9b572b-446d-4909-9423-b78d5de5bd2f</t>
+  </si>
+  <si>
+    <t>fcb26f74-0448-4c0a-b27a-1b5d41ae2a84</t>
+  </si>
+  <si>
+    <t>回收站功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>perm.document.update</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5202bd22-d7fc-4ea7-9f88-6c8af70b1853</t>
+  </si>
+  <si>
+    <t>文档重命名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>文档清除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>07032059-d5c8-4de5-818a-0dbea9aabb64</t>
+  </si>
+  <si>
+    <t>fe168b82-790e-4449-9e82-073567e46617</t>
+  </si>
+  <si>
+    <t>9c735d2b-5489-49df-9e84-eab1d1631772</t>
+  </si>
+  <si>
+    <t>还原文档</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>回收文档</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>清除文档</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>批量上传</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>批量下载</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>res.document.trash-in</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>res.document.trash-out</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>res.document.rename</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>res.document.purge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>res.file.upload.batch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>res.file.download.batch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a3933672-b2ad-4138-a15a-f029211d4419</t>
+  </si>
+  <si>
+    <t>c3c3c142-5031-4a7a-ab60-5e1b359015dc</t>
+  </si>
+  <si>
+    <t>913cf3b6-6103-4116-88a9-a4d4d3356438</t>
+  </si>
+  <si>
+    <t>a5e67097-ec0d-46fa-bc8c-4542e1df8b30</t>
+  </si>
+  <si>
+    <t>a3a90e59-54e9-41e4-abf9-a794e6c69d1c</t>
+  </si>
+  <si>
+    <t>2fb5e97c-bea8-452e-9339-909a51aa3c44</t>
+  </si>
+  <si>
+    <t>0f995149-fcf1-4ae3-821d-303f438c8b89</t>
+  </si>
+  <si>
+    <t>0988d65b-9df7-4d39-b5a5-91d982915503</t>
+  </si>
+  <si>
+    <t>act.document.trash-in</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DELETE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/document/trash</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>act.document.trash-out</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PUT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/document/rollback</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dea6f5b2-4c6d-4e01-a43f-f930ab932c37</t>
+  </si>
+  <si>
+    <t>adeb21a7-8b94-4051-811f-0081df45a378</t>
+  </si>
+  <si>
+    <t>87817410-b0b4-442c-b726-c7bbc290b544</t>
+  </si>
+  <si>
+    <t>f65171d4-f64a-4ffe-9cec-b7db778c6a45</t>
+  </si>
+  <si>
+    <t>4a4c608b-b570-4f9f-b5c7-f798e116f987</t>
+  </si>
+  <si>
+    <t>399d5994-0ab3-46d8-8ecd-6fcc2290fdde</t>
+  </si>
+  <si>
+    <t>491f6372-9d10-4d05-a98c-3d47f39df9dd</t>
+  </si>
+  <si>
+    <t>72c7a440-6f1b-4276-a725-d29ab408ef7c</t>
+  </si>
+  <si>
+    <t>act.document.rename</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/document/rename</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>act.document.purge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/document/purge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>act.file.upload.batch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/file/upload</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>act.file.download.batch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/file/download</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -587,7 +841,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -656,18 +910,6 @@
     <xf numFmtId="11" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -679,6 +921,21 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1021,10 +1278,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D6C9C3-8DFE-A442-A082-10767386D931}">
-  <dimension ref="A2:K38"/>
+  <dimension ref="A2:K64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="21"/>
@@ -1050,8 +1307,8 @@
       <c r="B2" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="33"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="38"/>
     </row>
     <row r="3" spans="1:9" s="23" customFormat="1">
       <c r="A3" s="24" t="s">
@@ -1119,556 +1376,1184 @@
       <c r="C7" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="30" t="s">
         <v>58</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="1" t="s">
+    <row r="8" spans="1:9">
+      <c r="A8" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" s="23" customFormat="1">
+      <c r="A11" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="23" customFormat="1">
+      <c r="A12" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C16" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="5" t="s">
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B17" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C17" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D17" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="7" t="s">
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B18" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C18" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D18" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E18" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="10" t="s">
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B19" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C19" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="D14" s="26" t="s">
+      <c r="D19" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E19" s="12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="10" t="s">
+    <row r="20" spans="1:9">
+      <c r="A20" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B20" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C20" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D20" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E20" s="12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="38" customFormat="1">
-      <c r="A16" s="10" t="s">
+    <row r="21" spans="1:9" s="34" customFormat="1">
+      <c r="A21" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B21" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C21" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D21" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="E16" s="35" t="s">
+      <c r="E21" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="F16" s="36"/>
-      <c r="G16" s="37"/>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="1" t="s">
+      <c r="F21" s="32"/>
+      <c r="G21" s="33"/>
+    </row>
+    <row r="22" spans="1:9" s="34" customFormat="1">
+      <c r="A22" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="E22" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="F22" s="32"/>
+      <c r="G22" s="33"/>
+    </row>
+    <row r="23" spans="1:9" s="34" customFormat="1">
+      <c r="A23" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="E23" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23" s="32"/>
+      <c r="G23" s="33"/>
+    </row>
+    <row r="24" spans="1:9" s="34" customFormat="1">
+      <c r="A24" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E24" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="F24" s="32"/>
+      <c r="G24" s="33"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C31" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="5" t="s">
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B32" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C32" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D32" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E32" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F32" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G32" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="H32" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I22" s="5" t="s">
+      <c r="I32" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
-      <c r="A23" s="7" t="s">
+    <row r="33" spans="1:11">
+      <c r="A33" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B33" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C33" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="D33" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E33" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F23" s="19" t="s">
+      <c r="F33" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G23" s="7" t="s">
+      <c r="G33" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H23" s="7" t="s">
+      <c r="H33" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I23" s="7" t="s">
+      <c r="I33" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
-      <c r="A24" s="10" t="s">
+    <row r="34" spans="1:11">
+      <c r="A34" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B24" s="16" t="str">
-        <f t="shared" ref="B24:B25" si="0">A35</f>
+      <c r="B34" s="16" t="str">
+        <f t="shared" ref="B34:B35" si="0">A53</f>
         <v>bfd1d794-bea3-4c79-aaaa-eceb53af3fcd</v>
       </c>
-      <c r="C24" s="16" t="str">
-        <f>A$14</f>
+      <c r="C34" s="16" t="str">
+        <f>A$19</f>
         <v>979ab118-e232-4595-a9cb-20b68e775fd7</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D34" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E34" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="13" t="s">
+      <c r="F34" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="G24" s="12" t="str">
-        <f>'DATA-PERM'!B14</f>
+      <c r="G34" s="12" t="str">
+        <f>'DATA-PERM'!B19</f>
         <v>读取文档</v>
       </c>
-      <c r="H24" s="12">
+      <c r="H34" s="12">
         <v>1</v>
       </c>
-      <c r="I24" s="12"/>
-      <c r="K24" s="14"/>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25" s="10" t="s">
+      <c r="I34" s="12"/>
+      <c r="K34" s="14"/>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="16" t="str">
+      <c r="B35" s="16" t="str">
         <f t="shared" si="0"/>
         <v>c2fd9e33-88e3-4f64-8755-c86c194158f7</v>
       </c>
-      <c r="C25" s="16" t="str">
-        <f>A$14</f>
+      <c r="C35" s="16" t="str">
+        <f>A$19</f>
         <v>979ab118-e232-4595-a9cb-20b68e775fd7</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D35" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="E35" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="F25" s="13" t="s">
+      <c r="F35" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="G25" s="12" t="s">
+      <c r="G35" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="H25" s="12">
+      <c r="H35" s="12">
         <v>1</v>
       </c>
-      <c r="I25" s="12"/>
-      <c r="K25" s="14"/>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="A26" s="10" t="s">
+      <c r="I35" s="12"/>
+      <c r="K35" s="14"/>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="16" t="str">
-        <f t="shared" ref="B26" si="1">A37</f>
+      <c r="B36" s="16" t="str">
+        <f t="shared" ref="B36" si="1">A55</f>
         <v>a9baa170-550b-44ee-8e32-b8eee8205483</v>
       </c>
-      <c r="C26" s="16" t="str">
-        <f>A15</f>
+      <c r="C36" s="16" t="str">
+        <f>A20</f>
         <v>be0f8b9b-bff1-4d38-af64-02efbb17a390</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D36" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="E36" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F26" s="13" t="s">
+      <c r="F36" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="G26" s="12" t="str">
-        <f>'DATA-PERM'!B15</f>
+      <c r="G36" s="12" t="str">
+        <f>'DATA-PERM'!B20</f>
         <v>搜索文档</v>
       </c>
-      <c r="H26" s="12">
+      <c r="H36" s="12">
         <v>1</v>
       </c>
-      <c r="I26" s="12"/>
-      <c r="K26" s="14"/>
-    </row>
-    <row r="27" spans="1:11" s="38" customFormat="1">
-      <c r="A27" s="10" t="s">
+      <c r="I36" s="12"/>
+      <c r="K36" s="14"/>
+    </row>
+    <row r="37" spans="1:11" s="34" customFormat="1">
+      <c r="A37" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B27" s="16" t="str">
-        <f>A38</f>
+      <c r="B37" s="16" t="str">
+        <f>A56</f>
         <v>e2348467-9bd1-4e6c-8f3b-f36a7491979b</v>
       </c>
-      <c r="C27" s="16" t="str">
-        <f>A16</f>
+      <c r="C37" s="16" t="str">
+        <f>A21</f>
         <v>086d23da-6542-46e2-88f9-e848d7df5200</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D37" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="E37" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="F27" s="13" t="s">
+      <c r="F37" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="G27" s="12" t="s">
+      <c r="G37" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="H27" s="12">
+      <c r="H37" s="12">
         <v>2</v>
       </c>
-      <c r="I27" s="12"/>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="A28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="3"/>
-      <c r="K28" s="14"/>
-    </row>
-    <row r="29" spans="1:11">
-      <c r="A29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="3"/>
-      <c r="K29" s="14"/>
-    </row>
-    <row r="30" spans="1:11">
-      <c r="A30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="3"/>
-      <c r="K30" s="14"/>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="A31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="3"/>
-      <c r="K31" s="14"/>
-    </row>
-    <row r="32" spans="1:11">
-      <c r="A32" s="1" t="s">
+      <c r="I37" s="12"/>
+    </row>
+    <row r="38" spans="1:11" s="34" customFormat="1">
+      <c r="A38" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="B38" s="16" t="str">
+        <f t="shared" ref="B38:B45" si="2">A57</f>
+        <v>a3933672-b2ad-4138-a15a-f029211d4419</v>
+      </c>
+      <c r="C38" s="16" t="str">
+        <f>A22</f>
+        <v>07032059-d5c8-4de5-818a-0dbea9aabb64</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="H38" s="12">
+        <v>12</v>
+      </c>
+      <c r="I38" s="12"/>
+    </row>
+    <row r="39" spans="1:11" s="34" customFormat="1">
+      <c r="A39" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="B39" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>c3c3c142-5031-4a7a-ab60-5e1b359015dc</v>
+      </c>
+      <c r="C39" s="16" t="str">
+        <f>A22</f>
+        <v>07032059-d5c8-4de5-818a-0dbea9aabb64</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="H39" s="12">
+        <v>8</v>
+      </c>
+      <c r="I39" s="12"/>
+    </row>
+    <row r="40" spans="1:11" s="34" customFormat="1">
+      <c r="A40" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="B40" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>913cf3b6-6103-4116-88a9-a4d4d3356438</v>
+      </c>
+      <c r="C40" s="16" t="str">
+        <f>A23</f>
+        <v>fe168b82-790e-4449-9e82-073567e46617</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="F40" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="H40" s="12">
+        <v>8</v>
+      </c>
+      <c r="I40" s="12"/>
+    </row>
+    <row r="41" spans="1:11" s="34" customFormat="1">
+      <c r="A41" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="B41" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>a5e67097-ec0d-46fa-bc8c-4542e1df8b30</v>
+      </c>
+      <c r="C41" s="16" t="str">
+        <f>A24</f>
+        <v>9c735d2b-5489-49df-9e84-eab1d1631772</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="G41" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="H41" s="12">
+        <v>12</v>
+      </c>
+      <c r="I41" s="12"/>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="B42" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>a3a90e59-54e9-41e4-abf9-a794e6c69d1c</v>
+      </c>
+      <c r="C42" s="16" t="str">
+        <f>A$25</f>
+        <v>4b398ad8-0d8c-4dab-8954-85130b86d973</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G42" s="12" t="str">
+        <f>B25</f>
+        <v>上传</v>
+      </c>
+      <c r="H42" s="12">
+        <v>4</v>
+      </c>
+      <c r="I42" s="12"/>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="B43" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>2fb5e97c-bea8-452e-9339-909a51aa3c44</v>
+      </c>
+      <c r="C43" s="16" t="str">
+        <f>A$25</f>
+        <v>4b398ad8-0d8c-4dab-8954-85130b86d973</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="F43" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="G43" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="H43" s="12">
+        <v>4</v>
+      </c>
+      <c r="I43" s="12"/>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="B44" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>0f995149-fcf1-4ae3-821d-303f438c8b89</v>
+      </c>
+      <c r="C44" s="16" t="str">
+        <f>A$26</f>
+        <v>7240209a-22d8-4ce5-a8a3-108c177354d9</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F44" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="G44" s="12" t="str">
+        <f>B26</f>
+        <v>下载</v>
+      </c>
+      <c r="H44" s="12">
         <v>1</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="I44" s="12"/>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="B45" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v>0988d65b-9df7-4d39-b5a5-91d982915503</v>
+      </c>
+      <c r="C45" s="16" t="str">
+        <f>A$26</f>
+        <v>7240209a-22d8-4ce5-a8a3-108c177354d9</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="F45" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="H45" s="12">
+        <v>1</v>
+      </c>
+      <c r="I45" s="12"/>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" s="14"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="3"/>
+      <c r="K46" s="14"/>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" s="14"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="3"/>
+      <c r="K47" s="14"/>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" s="14"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="3"/>
+      <c r="K48" s="14"/>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" s="14"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="3"/>
+      <c r="K49" s="14"/>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="30" t="s">
+      <c r="C50" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="31"/>
-      <c r="K32" s="31"/>
-    </row>
-    <row r="33" spans="1:11">
-      <c r="A33" s="5" t="s">
+      <c r="D50" s="36"/>
+      <c r="E50" s="36"/>
+      <c r="F50" s="36"/>
+      <c r="G50" s="36"/>
+      <c r="H50" s="36"/>
+      <c r="I50" s="36"/>
+      <c r="J50" s="36"/>
+      <c r="K50" s="36"/>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="A51" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B51" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C51" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D51" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="E51" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="F51" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G33" s="20" t="s">
+      <c r="G51" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="H33" s="20" t="s">
+      <c r="H51" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="I33" s="20" t="s">
+      <c r="I51" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="J33" s="5" t="s">
+      <c r="J51" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="K33" s="5" t="s">
+      <c r="K51" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
-      <c r="A34" s="7" t="s">
+    <row r="52" spans="1:11">
+      <c r="A52" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B52" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C52" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D34" s="19" t="s">
+      <c r="D52" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E34" s="9" t="s">
+      <c r="E52" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="F34" s="9" t="s">
+      <c r="F52" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="7" t="s">
+      <c r="G52" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="H34" s="7" t="s">
+      <c r="H52" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="I34" s="7" t="s">
+      <c r="I52" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="7" t="s">
+      <c r="J52" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="K34" s="7" t="s">
+      <c r="K52" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
-      <c r="A35" s="29" t="s">
+    <row r="53" spans="1:11">
+      <c r="A53" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="B35" s="12" t="str">
-        <f>'DATA-PERM'!B14</f>
+      <c r="B53" s="12" t="str">
+        <f>'DATA-PERM'!B19</f>
         <v>读取文档</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C53" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D35" s="13" t="s">
+      <c r="D53" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="E35" s="35" t="s">
+      <c r="E53" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="F35" s="12" t="s">
+      <c r="F53" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G35" s="12">
+      <c r="G53" s="12">
         <v>1</v>
       </c>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="11"/>
-    </row>
-    <row r="36" spans="1:11">
-      <c r="A36" s="29" t="s">
+      <c r="H53" s="12"/>
+      <c r="I53" s="12"/>
+      <c r="J53" s="11"/>
+      <c r="K53" s="11"/>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B54" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C54" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="13" t="s">
+      <c r="D54" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="E36" s="35" t="s">
+      <c r="E54" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="F36" s="12" t="s">
+      <c r="F54" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G36" s="12">
+      <c r="G54" s="12">
         <v>1</v>
       </c>
-      <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="11"/>
-    </row>
-    <row r="37" spans="1:11">
-      <c r="A37" s="29" t="s">
+      <c r="H54" s="12"/>
+      <c r="I54" s="12"/>
+      <c r="J54" s="11"/>
+      <c r="K54" s="11"/>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="B37" s="12" t="str">
-        <f>'DATA-PERM'!B15</f>
+      <c r="B55" s="12" t="str">
+        <f>'DATA-PERM'!B20</f>
         <v>搜索文档</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C55" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D37" s="13" t="s">
+      <c r="D55" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="E37" s="35" t="s">
+      <c r="E55" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="F37" s="12" t="s">
+      <c r="F55" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G37" s="12">
+      <c r="G55" s="12">
         <v>1</v>
       </c>
-      <c r="H37" s="12"/>
-      <c r="I37" s="12"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="11"/>
-    </row>
-    <row r="38" spans="1:11" s="38" customFormat="1">
-      <c r="A38" s="10" t="s">
+      <c r="H55" s="12"/>
+      <c r="I55" s="12"/>
+      <c r="J55" s="11"/>
+      <c r="K55" s="11"/>
+    </row>
+    <row r="56" spans="1:11" s="34" customFormat="1">
+      <c r="A56" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="B38" s="12" t="s">
+      <c r="B56" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C56" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D38" s="13" t="s">
+      <c r="D56" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="E38" s="35" t="s">
+      <c r="E56" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="F38" s="12" t="s">
+      <c r="F56" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G38" s="12">
+      <c r="G56" s="12">
         <v>1</v>
       </c>
-      <c r="H38" s="12"/>
-      <c r="I38" s="12"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="11"/>
+      <c r="H56" s="12"/>
+      <c r="I56" s="12"/>
+      <c r="J56" s="11"/>
+      <c r="K56" s="11"/>
+    </row>
+    <row r="57" spans="1:11" s="34" customFormat="1">
+      <c r="A57" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D57" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="E57" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="F57" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G57" s="12">
+        <v>12</v>
+      </c>
+      <c r="H57" s="12"/>
+      <c r="I57" s="12"/>
+      <c r="J57" s="11"/>
+      <c r="K57" s="11"/>
+    </row>
+    <row r="58" spans="1:11" s="34" customFormat="1">
+      <c r="A58" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D58" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="E58" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="F58" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G58" s="12">
+        <v>8</v>
+      </c>
+      <c r="H58" s="12"/>
+      <c r="I58" s="12"/>
+      <c r="J58" s="11"/>
+      <c r="K58" s="11"/>
+    </row>
+    <row r="59" spans="1:11" s="34" customFormat="1">
+      <c r="A59" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D59" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E59" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="F59" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G59" s="12">
+        <v>8</v>
+      </c>
+      <c r="H59" s="12"/>
+      <c r="I59" s="12"/>
+      <c r="J59" s="11"/>
+      <c r="K59" s="11"/>
+    </row>
+    <row r="60" spans="1:11" s="34" customFormat="1">
+      <c r="A60" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B60" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D60" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E60" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="F60" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G60" s="12">
+        <v>12</v>
+      </c>
+      <c r="H60" s="12"/>
+      <c r="I60" s="12"/>
+      <c r="J60" s="11"/>
+      <c r="K60" s="11"/>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="A61" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B61" s="12" t="str">
+        <f>B25</f>
+        <v>上传</v>
+      </c>
+      <c r="C61" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D61" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E61" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F61" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G61" s="12">
+        <v>4</v>
+      </c>
+      <c r="H61" s="12"/>
+      <c r="I61" s="12"/>
+      <c r="J61" s="11"/>
+      <c r="K61" s="11"/>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B62" s="12" t="str">
+        <f>G43</f>
+        <v>批量上传</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D62" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="E62" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F62" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G62" s="12">
+        <v>4</v>
+      </c>
+      <c r="H62" s="12"/>
+      <c r="I62" s="12"/>
+      <c r="J62" s="11"/>
+      <c r="K62" s="11"/>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="B63" s="12" t="str">
+        <f>B26</f>
+        <v>下载</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D63" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="E63" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F63" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G63" s="12">
+        <v>1</v>
+      </c>
+      <c r="H63" s="12"/>
+      <c r="I63" s="12"/>
+      <c r="J63" s="11"/>
+      <c r="K63" s="11"/>
+    </row>
+    <row r="64" spans="1:11">
+      <c r="A64" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="B64" s="12" t="str">
+        <f>G45</f>
+        <v>批量下载</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D64" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="E64" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F64" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G64" s="12">
+        <v>1</v>
+      </c>
+      <c r="H64" s="12"/>
+      <c r="I64" s="12"/>
+      <c r="J64" s="11"/>
+      <c r="K64" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C16:E16"/>
     <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C32:K32"/>
+    <mergeCell ref="C50:K50"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>